<commit_message>
Actualización: cambios en Pen_Sales.py y hoja de datos
</commit_message>
<xml_diff>
--- a/Data/Pen Sales Data.xlsx
+++ b/Data/Pen Sales Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28803"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alice/Desktop/Course_Materials/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF10E04D-C46A-CB42-950C-0B504C1B54A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9785123-FC76-4CF6-AA29-4AD223960C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="500" windowWidth="28040" windowHeight="16000" xr2:uid="{88CB5200-0D19-2446-86AC-C4FBD1C615F9}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Pen Sales" sheetId="1" r:id="rId1"/>
     <sheet name="Pen Costs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,9 +24,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,11 +37,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="43">
   <si>
     <t>Customer</t>
   </si>
   <si>
+    <t>Item</t>
+  </si>
+  <si>
     <t>Pen Cost</t>
   </si>
   <si>
@@ -54,106 +60,112 @@
     <t>Review</t>
   </si>
   <si>
-    <t>Item</t>
-  </si>
-  <si>
     <t>Ballpoint Pens</t>
   </si>
   <si>
+    <t>DoodleWithMe|I love the way this pen writes, but unfortunately it has a tendency to leak if left unused for too long. It's important to keep it capped when not in use.</t>
+  </si>
+  <si>
     <t>Sharpies</t>
   </si>
   <si>
+    <t>ScribbleMaster|The classic Sharpie marker has a bold, permanent ink that works on almost any surface. It's perfect for labeling, drawing, or writing in a variety of settings.</t>
+  </si>
+  <si>
     <t>Ballpoint Pens (Bold)</t>
   </si>
   <si>
+    <t>PenPalForever|The retractable ballpoint pen has a durable, metal clip and a sturdy design. It writes with a consistent flow and is a reliable choice for everyday use.</t>
+  </si>
+  <si>
     <t>Gel Pens</t>
   </si>
   <si>
+    <t>TheWriteWay|This gel pen has a comfortable grip and writes with vibrant, consistent ink. It's perfect for taking notes or writing in a journal.</t>
+  </si>
+  <si>
     <t>Rollerball Pens</t>
   </si>
   <si>
+    <t>PenAndPaperPerson|The rollerball pen has a smooth, fluid feel and creates bold, expressive lines. It's a great option for artists and writers who want to add personality to their work.</t>
+  </si>
+  <si>
     <t>Gel Pens (Pastel)</t>
   </si>
   <si>
+    <t>SmoothOperatorPen|This gel pen writes smoothly with a bold, vibrant ink that stands out on paper. It's perfect for adding a pop of color to notes or artwork.</t>
+  </si>
+  <si>
+    <t>InkStainedFingers|This pen is prone to leaking and can create a mess if not handled carefully. It writes well, but may not be the best option for those on-the-go.</t>
+  </si>
+  <si>
+    <t>BoldInkWriter|Unfortunately, this pen has a tendency to spill ink if jostled or dropped. It writes smoothly, but may not be the most practical choice for everyday use.</t>
+  </si>
+  <si>
+    <t>PenmanshipPro|The gel pen has a comfortable grip and writes with a consistent flow. The ink dries quickly and is smudge-proof, making it a great choice for left-handed writers.</t>
+  </si>
+  <si>
+    <t>GelPenGuru|This retractable gel pen has a fine point that allows for precise writing and drawing. The ink is water-resistant and fade-proof, ensuring long-lasting results.</t>
+  </si>
+  <si>
+    <t>FinePointFan|Be careful with this pen, as it has been known to leak if not stored upright. That being said, it writes with a bold ink that stands out on paper.</t>
+  </si>
+  <si>
+    <t>SignatureStylePen|The retractable ballpoint pen is convenient and easy to use. It writes cleanly and is a good choice for those who prefer a no-fuss writing instrument.</t>
+  </si>
+  <si>
+    <t>BoldAndBeautifulPen|</t>
+  </si>
+  <si>
+    <t>RollerballRider|The ink in this pen has a tendency to leak out and create smudges on paper. It's a shame, because the pen itself is comfortable to hold and writes well.</t>
+  </si>
+  <si>
+    <t>BallpointBandit|This ballpoint pen has a sleek design and writes smoothly with a consistent flow. It's a great option for everyday use and is available in a variety of colors.</t>
+  </si>
+  <si>
+    <t>TwistAndWriteUser|The ink in this pen can sometimes leak out of the tip, creating a mess on paper. However, the pen is comfortable to hold and writes with a smooth flow.</t>
+  </si>
+  <si>
+    <t>ThePenWhisperer|</t>
+  </si>
+  <si>
+    <t>InkFlowFollower|I was disappointed to find that this pen leaked after only a few uses. The ink is nice, but the potential for spills makes it difficult to recommend.</t>
+  </si>
+  <si>
+    <t>ThePenAndInkLady|This ballpoint pen has a comfortable grip and a medium point that creates clear, easy-to-read lines. It's a great option for writing notes or letters.</t>
+  </si>
+  <si>
+    <t>WritingInstrumentsFan|This pen is great for writing, but it's not very travel-friendly as it has a tendency to spill ink in transit. It's best to use it in a stationary setting.</t>
+  </si>
+  <si>
+    <t>PenPrecisionPro|The retractable Sharpie marker is convenient and easy to use. It has a durable tip and writes with a consistent flow.</t>
+  </si>
+  <si>
+    <t>InkCollector|The ballpoint pen is lightweight and comfortable to hold. It writes smoothly and has a medium point that creates a clear, legible line.</t>
+  </si>
+  <si>
+    <t>PenToPaperPersonality|</t>
+  </si>
+  <si>
+    <t>SmoothWritingScribe|This fine point Sharpie marker has a precise tip that allows for detailed work. The ink dries quickly and is resistant to water and fading.</t>
+  </si>
+  <si>
+    <t>ThePenmanshipPundit|This pen writes smoothly and delivers a crisp line. The ink dries quickly and is smudge-proof, making it a great choice for left-handed writers.</t>
+  </si>
+  <si>
+    <t>15/6/2023</t>
+  </si>
+  <si>
+    <t>13/5/2023</t>
+  </si>
+  <si>
+    <t>14/2/2023</t>
+  </si>
+  <si>
     <t>Pen</t>
   </si>
   <si>
     <t>Cost</t>
-  </si>
-  <si>
-    <t>DoodleWithMe|I love the way this pen writes, but unfortunately it has a tendency to leak if left unused for too long. It's important to keep it capped when not in use.</t>
-  </si>
-  <si>
-    <t>ScribbleMaster|The classic Sharpie marker has a bold, permanent ink that works on almost any surface. It's perfect for labeling, drawing, or writing in a variety of settings.</t>
-  </si>
-  <si>
-    <t>PenPalForever|The retractable ballpoint pen has a durable, metal clip and a sturdy design. It writes with a consistent flow and is a reliable choice for everyday use.</t>
-  </si>
-  <si>
-    <t>TheWriteWay|This gel pen has a comfortable grip and writes with vibrant, consistent ink. It's perfect for taking notes or writing in a journal.</t>
-  </si>
-  <si>
-    <t>PenAndPaperPerson|The rollerball pen has a smooth, fluid feel and creates bold, expressive lines. It's a great option for artists and writers who want to add personality to their work.</t>
-  </si>
-  <si>
-    <t>SmoothOperatorPen|This gel pen writes smoothly with a bold, vibrant ink that stands out on paper. It's perfect for adding a pop of color to notes or artwork.</t>
-  </si>
-  <si>
-    <t>InkStainedFingers|This pen is prone to leaking and can create a mess if not handled carefully. It writes well, but may not be the best option for those on-the-go.</t>
-  </si>
-  <si>
-    <t>BoldInkWriter|Unfortunately, this pen has a tendency to spill ink if jostled or dropped. It writes smoothly, but may not be the most practical choice for everyday use.</t>
-  </si>
-  <si>
-    <t>PenmanshipPro|The gel pen has a comfortable grip and writes with a consistent flow. The ink dries quickly and is smudge-proof, making it a great choice for left-handed writers.</t>
-  </si>
-  <si>
-    <t>GelPenGuru|This retractable gel pen has a fine point that allows for precise writing and drawing. The ink is water-resistant and fade-proof, ensuring long-lasting results.</t>
-  </si>
-  <si>
-    <t>FinePointFan|Be careful with this pen, as it has been known to leak if not stored upright. That being said, it writes with a bold ink that stands out on paper.</t>
-  </si>
-  <si>
-    <t>SignatureStylePen|The retractable ballpoint pen is convenient and easy to use. It writes cleanly and is a good choice for those who prefer a no-fuss writing instrument.</t>
-  </si>
-  <si>
-    <t>BoldAndBeautifulPen|</t>
-  </si>
-  <si>
-    <t>RollerballRider|The ink in this pen has a tendency to leak out and create smudges on paper. It's a shame, because the pen itself is comfortable to hold and writes well.</t>
-  </si>
-  <si>
-    <t>BallpointBandit|This ballpoint pen has a sleek design and writes smoothly with a consistent flow. It's a great option for everyday use and is available in a variety of colors.</t>
-  </si>
-  <si>
-    <t>TwistAndWriteUser|The ink in this pen can sometimes leak out of the tip, creating a mess on paper. However, the pen is comfortable to hold and writes with a smooth flow.</t>
-  </si>
-  <si>
-    <t>ThePenWhisperer|</t>
-  </si>
-  <si>
-    <t>InkFlowFollower|I was disappointed to find that this pen leaked after only a few uses. The ink is nice, but the potential for spills makes it difficult to recommend.</t>
-  </si>
-  <si>
-    <t>ThePenAndInkLady|This ballpoint pen has a comfortable grip and a medium point that creates clear, easy-to-read lines. It's a great option for writing notes or letters.</t>
-  </si>
-  <si>
-    <t>WritingInstrumentsFan|This pen is great for writing, but it's not very travel-friendly as it has a tendency to spill ink in transit. It's best to use it in a stationary setting.</t>
-  </si>
-  <si>
-    <t>PenPrecisionPro|The retractable Sharpie marker is convenient and easy to use. It has a durable tip and writes with a consistent flow.</t>
-  </si>
-  <si>
-    <t>InkCollector|The ballpoint pen is lightweight and comfortable to hold. It writes smoothly and has a medium point that creates a clear, legible line.</t>
-  </si>
-  <si>
-    <t>PenToPaperPersonality|</t>
-  </si>
-  <si>
-    <t>SmoothWritingScribe|This fine point Sharpie marker has a precise tip that allows for detailed work. The ink dries quickly and is resistant to water and fading.</t>
-  </si>
-  <si>
-    <t>ThePenmanshipPundit|This pen writes smoothly and delivers a crisp line. The ink dries quickly and is smudge-proof, making it a great choice for left-handed writers.</t>
   </si>
 </sst>
 </file>
@@ -164,7 +176,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -216,16 +228,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -538,46 +553,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B65F30A-E2C2-D84E-BD5E-139BBF0CA3F0}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="155.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="155.125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>5201</v>
       </c>
@@ -597,16 +614,16 @@
         <v>45049</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <f>A2+1</f>
         <v>5202</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2">
         <v>12.99</v>
@@ -621,16 +638,16 @@
         <v>45050</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <f t="shared" ref="A4:A26" si="0">A3+1</f>
         <v>5203</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2">
         <v>6.95</v>
@@ -645,16 +662,16 @@
         <v>45048</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>5204</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2">
         <v>5.99</v>
@@ -669,16 +686,16 @@
         <v>45050</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5205</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2">
         <v>12.99</v>
@@ -693,16 +710,16 @@
         <v>45049</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5206</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2">
         <v>14.99</v>
@@ -717,16 +734,16 @@
         <v>45050</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>5207</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2">
         <v>12.99</v>
@@ -741,16 +758,16 @@
         <v>45049</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>5208</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2">
         <v>12.99</v>
@@ -765,16 +782,16 @@
         <v>45053</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>5209</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2">
         <v>5.99</v>
@@ -789,16 +806,16 @@
         <v>45052</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>5210</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C11" s="2">
         <v>14.99</v>
@@ -813,16 +830,16 @@
         <v>45048</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>5211</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2">
         <v>6.95</v>
@@ -837,16 +854,16 @@
         <v>45050</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>5212</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2">
         <v>6.95</v>
@@ -861,16 +878,16 @@
         <v>45053</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>5213</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2">
         <v>12.99</v>
@@ -885,16 +902,16 @@
         <v>45049</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>5214</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C15" s="2">
         <v>12.99</v>
@@ -909,10 +926,10 @@
         <v>45053</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>5215</v>
@@ -933,16 +950,16 @@
         <v>45049</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>5216</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C17" s="2">
         <v>5.99</v>
@@ -957,16 +974,16 @@
         <v>45050</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>5217</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C18" s="2">
         <v>12.99</v>
@@ -981,16 +998,16 @@
         <v>45050</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>5218</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C19" s="2">
         <v>14.99</v>
@@ -1005,10 +1022,10 @@
         <v>45049</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>5219</v>
@@ -1029,16 +1046,16 @@
         <v>45053</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>5220</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C21" s="2">
         <v>5.99</v>
@@ -1053,16 +1070,16 @@
         <v>45053</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>5221</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C22" s="2">
         <v>12.99</v>
@@ -1077,10 +1094,10 @@
         <v>45051</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>5222</v>
@@ -1101,16 +1118,16 @@
         <v>45051</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>5223</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C24" s="2">
         <v>6.95</v>
@@ -1125,16 +1142,16 @@
         <v>45052</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>5224</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C25" s="2">
         <v>12.99</v>
@@ -1142,23 +1159,23 @@
       <c r="D25" s="2">
         <v>2.99</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="6">
         <v>45048</v>
       </c>
       <c r="F25" s="3">
         <v>45052</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>5225</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C26" s="2">
         <v>6.95</v>
@@ -1166,14 +1183,613 @@
       <c r="D26" s="2">
         <v>2.99</v>
       </c>
-      <c r="E26" s="3">
-        <v>45048</v>
+      <c r="E26" s="6">
+        <v>45047</v>
       </c>
       <c r="F26" s="3">
         <v>45053</v>
       </c>
       <c r="G26" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>5226</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="2">
+        <v>5.99</v>
+      </c>
+      <c r="D27" s="2">
+        <v>2.99</v>
+      </c>
+      <c r="E27" s="6">
+        <v>45021</v>
+      </c>
+      <c r="F27" s="3">
+        <v>45049</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <f>A27+1</f>
+        <v>5227</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="2">
+        <v>12.99</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="6">
+        <v>45112</v>
+      </c>
+      <c r="F28" s="3">
+        <v>45050</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <f t="shared" ref="A29:A51" si="1">A28+1</f>
+        <v>5228</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="2">
+        <v>6.95</v>
+      </c>
+      <c r="D29" s="2">
+        <v>4.99</v>
+      </c>
+      <c r="E29" s="6">
+        <v>45205</v>
+      </c>
+      <c r="F29" s="3">
+        <v>45048</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <f t="shared" si="1"/>
+        <v>5229</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="2">
+        <v>5.99</v>
+      </c>
+      <c r="D30" s="2">
+        <v>2.99</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" s="3">
+        <v>45050</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
+        <f t="shared" si="1"/>
+        <v>5230</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="2">
+        <v>12.99</v>
+      </c>
+      <c r="D31" s="2">
+        <v>1.99</v>
+      </c>
+      <c r="E31" s="3">
+        <v>45204</v>
+      </c>
+      <c r="F31" s="3">
+        <v>45049</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32">
+        <f t="shared" si="1"/>
+        <v>5231</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="2">
+        <v>14.99</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1.99</v>
+      </c>
+      <c r="E32" s="3">
+        <v>45052</v>
+      </c>
+      <c r="F32" s="3">
+        <v>45050</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <f t="shared" si="1"/>
+        <v>5232</v>
+      </c>
+      <c r="B33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="2">
+        <v>12.99</v>
+      </c>
+      <c r="D33" s="2">
+        <v>1.99</v>
+      </c>
+      <c r="E33" s="3">
+        <v>45051</v>
+      </c>
+      <c r="F33" s="3">
+        <v>45049</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34">
+        <f t="shared" si="1"/>
+        <v>5233</v>
+      </c>
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="2">
+        <v>12.99</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1.99</v>
+      </c>
+      <c r="E34" s="3">
+        <v>45050</v>
+      </c>
+      <c r="F34" s="3">
+        <v>45053</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35">
+        <f t="shared" si="1"/>
+        <v>5234</v>
+      </c>
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="2">
+        <v>5.99</v>
+      </c>
+      <c r="D35" s="2">
+        <v>2.99</v>
+      </c>
+      <c r="E35" s="6">
+        <v>44988</v>
+      </c>
+      <c r="F35" s="3">
+        <v>45052</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36">
+        <f t="shared" si="1"/>
+        <v>5235</v>
+      </c>
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="2">
+        <v>14.99</v>
+      </c>
+      <c r="D36" s="2">
+        <v>4.99</v>
+      </c>
+      <c r="E36" s="6">
+        <v>45080</v>
+      </c>
+      <c r="F36" s="3">
+        <v>45048</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37">
+        <f t="shared" si="1"/>
+        <v>5236</v>
+      </c>
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="2">
+        <v>6.95</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0</v>
+      </c>
+      <c r="E37" s="6">
+        <v>45141</v>
+      </c>
+      <c r="F37" s="3">
+        <v>45050</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38">
+        <f t="shared" si="1"/>
+        <v>5237</v>
+      </c>
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="2">
+        <v>6.95</v>
+      </c>
+      <c r="D38" s="2">
+        <v>2.99</v>
+      </c>
+      <c r="E38" s="6">
+        <v>45172</v>
+      </c>
+      <c r="F38" s="3">
+        <v>45053</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39">
+        <f t="shared" si="1"/>
+        <v>5238</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="2">
+        <v>12.99</v>
+      </c>
+      <c r="D39" s="2">
+        <v>1.99</v>
+      </c>
+      <c r="E39" s="6">
+        <v>45202</v>
+      </c>
+      <c r="F39" s="3">
+        <v>45049</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40">
+        <f t="shared" si="1"/>
+        <v>5239</v>
+      </c>
+      <c r="B40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="2">
+        <v>12.99</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1.99</v>
+      </c>
+      <c r="E40" s="6">
+        <v>45235</v>
+      </c>
+      <c r="F40" s="3">
+        <v>45053</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.75">
+      <c r="A41">
+        <f t="shared" si="1"/>
+        <v>5240</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="2">
+        <v>5.99</v>
+      </c>
+      <c r="D41" s="2">
+        <v>1.99</v>
+      </c>
+      <c r="E41" s="6">
+        <v>45265</v>
+      </c>
+      <c r="F41" s="4">
+        <v>45049</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42">
+        <f t="shared" si="1"/>
+        <v>5241</v>
+      </c>
+      <c r="B42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="2">
+        <v>5.99</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0</v>
+      </c>
+      <c r="E42" s="6" t="s">
         <v>39</v>
+      </c>
+      <c r="F42" s="3">
+        <v>45050</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43">
+        <f t="shared" si="1"/>
+        <v>5242</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="2">
+        <v>12.99</v>
+      </c>
+      <c r="D43" s="2">
+        <v>2.99</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" s="3">
+        <v>45050</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15.75">
+      <c r="A44">
+        <f t="shared" si="1"/>
+        <v>5243</v>
+      </c>
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="2">
+        <v>14.99</v>
+      </c>
+      <c r="D44" s="2">
+        <v>4.99</v>
+      </c>
+      <c r="E44" s="6">
+        <v>45110</v>
+      </c>
+      <c r="F44" s="4">
+        <v>45049</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45">
+        <f t="shared" si="1"/>
+        <v>5244</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="2">
+        <v>5.99</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0</v>
+      </c>
+      <c r="E45" s="6">
+        <v>45177</v>
+      </c>
+      <c r="F45" s="3">
+        <v>45053</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46">
+        <f t="shared" si="1"/>
+        <v>5245</v>
+      </c>
+      <c r="B46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="2">
+        <v>5.99</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0</v>
+      </c>
+      <c r="E46" s="6">
+        <v>45174</v>
+      </c>
+      <c r="F46" s="3">
+        <v>45053</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15.75">
+      <c r="A47">
+        <f t="shared" si="1"/>
+        <v>5246</v>
+      </c>
+      <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="2">
+        <v>12.99</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1.99</v>
+      </c>
+      <c r="E47" s="6">
+        <v>45201</v>
+      </c>
+      <c r="F47" s="4">
+        <v>45051</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15.75">
+      <c r="A48">
+        <f t="shared" si="1"/>
+        <v>5247</v>
+      </c>
+      <c r="B48" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="2">
+        <v>5.99</v>
+      </c>
+      <c r="D48" s="2">
+        <v>1.99</v>
+      </c>
+      <c r="E48" s="6">
+        <v>45232</v>
+      </c>
+      <c r="F48" s="4">
+        <v>45051</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49">
+        <f t="shared" si="1"/>
+        <v>5248</v>
+      </c>
+      <c r="B49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="2">
+        <v>6.95</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0</v>
+      </c>
+      <c r="E49" s="6">
+        <v>44987</v>
+      </c>
+      <c r="F49" s="3">
+        <v>45052</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50">
+        <f t="shared" si="1"/>
+        <v>5249</v>
+      </c>
+      <c r="B50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="2">
+        <v>12.99</v>
+      </c>
+      <c r="D50" s="2">
+        <v>2.99</v>
+      </c>
+      <c r="E50" s="6">
+        <v>45171</v>
+      </c>
+      <c r="F50" s="3">
+        <v>45052</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51">
+        <f t="shared" si="1"/>
+        <v>5250</v>
+      </c>
+      <c r="B51" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="2">
+        <v>6.95</v>
+      </c>
+      <c r="D51" s="2">
+        <v>2.99</v>
+      </c>
+      <c r="E51" s="6">
+        <v>45052</v>
+      </c>
+      <c r="F51" s="3">
+        <v>45053</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1187,21 +1803,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="5" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1209,41 +1825,41 @@
         <v>5.99</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
         <v>12.99</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1">
         <v>6.95</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1">
         <v>5.99</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1">
         <v>12.99</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1">
         <v>14.99</v>
@@ -1255,6 +1871,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100AD83AFDB133AE84091E51804354FA7EE" ma:contentTypeVersion="8" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="f49275ace62bf5fa599342d318323630">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1bb583d6-7de5-4467-bb06-9aeb8738f185" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0d007ce636fb2ce637e66dc94a6f9197" ns2:_="">
     <xsd:import namespace="1bb583d6-7de5-4467-bb06-9aeb8738f185"/>
@@ -1422,15 +2047,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1438,11 +2054,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD506EFA-CF68-4EB5-A8AA-F6E42D705E41}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F82D2F-E708-4223-A587-34EE88DDC2ED}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F82D2F-E708-4223-A587-34EE88DDC2ED}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD506EFA-CF68-4EB5-A8AA-F6E42D705E41}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>